<commit_message>
updated readme and issue log
</commit_message>
<xml_diff>
--- a/docs/issue_log/issue_log.xlsx
+++ b/docs/issue_log/issue_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="37">
   <si>
     <t>issue no.</t>
   </si>
@@ -74,14 +74,129 @@
   </si>
   <si>
     <t>all pages</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>top image</t>
+  </si>
+  <si>
+    <t>update better image with special font</t>
+  </si>
+  <si>
+    <t>top bar menu</t>
+  </si>
+  <si>
+    <t>add media break point - increase to 150% at larger screen size</t>
+  </si>
+  <si>
+    <t>turn off text decoration for hyperlink</t>
+  </si>
+  <si>
+    <t>about</t>
+  </si>
+  <si>
+    <t>add large image stretch across the width</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">add content about you to demonstrate your </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>personality,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">skills </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">and/or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>interests</t>
+    </r>
+  </si>
+  <si>
+    <t>portfolio</t>
+  </si>
+  <si>
+    <t>update image and component alignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Links to professional accounts such as Github and LinkedIn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">place comments in the CSS and HTML code to identify each </t>
+  </si>
+  <si>
+    <t>Implement Subresource Integrity (SRI) to enable browsers to verify that resources they fetch are delivered without unexpected manipulation.</t>
+  </si>
+  <si>
+    <t>Tech stack (e.g. html, css, deployment platform, etc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Functionality / features
+</t>
+  </si>
+  <si>
+    <t>Sitemap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -97,7 +212,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -105,13 +220,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,214 +557,398 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="42" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="4">
         <v>43727</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="4">
+        <v>43728</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="4">
+        <v>43728</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="4">
         <v>43728</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="F9" s="4">
+        <v>43727</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
+      <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14">
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="4">
+        <v>43728</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="4">
+        <v>43728</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16">
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="4">
+        <v>43728</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17">
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18">
+      <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="B18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
         <v>23</v>
       </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
created screenshot of issue log and update readme.md
</commit_message>
<xml_diff>
--- a/docs/issue_log/issue_log.xlsx
+++ b/docs/issue_log/issue_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>issue no.</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>Sitemap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y </t>
+  </si>
+  <si>
+    <t>readme</t>
   </si>
 </sst>
 </file>
@@ -559,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -660,8 +666,12 @@
       <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="4">
+        <v>43729</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
@@ -674,8 +684,12 @@
       <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="4">
+        <v>43729</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
@@ -688,8 +702,12 @@
       <c r="D7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="4">
+        <v>43729</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
@@ -842,8 +860,12 @@
       <c r="D16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="4">
+        <v>43730</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
@@ -877,7 +899,9 @@
       <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="3" t="s">
         <v>35</v>
@@ -889,7 +913,9 @@
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="3" t="s">
         <v>34</v>
@@ -901,7 +927,9 @@
       <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="3" t="s">
         <v>36</v>

</xml_diff>